<commit_message>
commit 3 ( cambio de variable en Hospedaje)
</commit_message>
<xml_diff>
--- a/Avance.xlsx
+++ b/Avance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
   <si>
     <t>Package Entidad</t>
   </si>
@@ -118,13 +118,19 @@
   </si>
   <si>
     <t>Hospedajes y monto</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Autogenerado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +140,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -454,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -510,6 +533,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,14 +851,16 @@
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="19" t="s">
         <v>0</v>
@@ -848,58 +879,88 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="D3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="18"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="D4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="18"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
         <v>7</v>
       </c>
@@ -911,73 +972,127 @@
         <v>5</v>
       </c>
       <c r="F11" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="H11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="I11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="J11" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="K11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="L11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="M11" s="24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
       <c r="D15" s="25" t="s">
@@ -986,25 +1101,26 @@
       <c r="E15" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="25"/>
+      <c r="G15" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="H15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="I15" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="J15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="K15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="4"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1013,13 +1129,14 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="4"/>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1028,98 +1145,99 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="9"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28"/>
       <c r="B23" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="13"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29"/>
       <c r="B27" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="13"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="29"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="13"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">

</xml_diff>